<commit_message>
I added more fish
</commit_message>
<xml_diff>
--- a/fishdata.xlsx
+++ b/fishdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>id</t>
   </si>
@@ -28,6 +28,12 @@
   </si>
   <si>
     <t>fatfish</t>
+  </si>
+  <si>
+    <t>longfish</t>
+  </si>
+  <si>
+    <t>shortfish</t>
   </si>
 </sst>
 </file>
@@ -366,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,6 +411,50 @@
       </c>
       <c r="C3">
         <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>